<commit_message>
refactor(parser): allow only => and -> as separators for user-uploaded words
</commit_message>
<xml_diff>
--- a/assets/examples/example.xlsx
+++ b/assets/examples/example.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>sí</t>
   </si>
@@ -40,6 +40,42 @@
   </si>
   <si>
     <t>dog</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>uno</t>
+  </si>
+  <si>
+    <t>lifetime</t>
+  </si>
+  <si>
+    <t>toda la vida</t>
+  </si>
+  <si>
+    <t>see you later</t>
+  </si>
+  <si>
+    <t>hasta luego</t>
+  </si>
+  <si>
+    <t>how are you</t>
+  </si>
+  <si>
+    <t>qué tal</t>
+  </si>
+  <si>
+    <t>bank, bench</t>
+  </si>
+  <si>
+    <t>banco</t>
+  </si>
+  <si>
+    <t>light</t>
+  </si>
+  <si>
+    <t>luz, ligero</t>
   </si>
 </sst>
 </file>
@@ -385,16 +421,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -403,30 +443,83 @@
     </row>
     <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>